<commit_message>
Added add cell value function.
</commit_message>
<xml_diff>
--- a/output/TestBook.xlsx
+++ b/output/TestBook.xlsx
@@ -421,7 +421,15 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>New Data</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added new sheet function.
</commit_message>
<xml_diff>
--- a/output/TestBook.xlsx
+++ b/output/TestBook.xlsx
@@ -7,8 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Introduction_Modified" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="New Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Introduction_Modified" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -414,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="B1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,7 +424,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>New Data</t>
         </is>
@@ -450,4 +451,22 @@
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Skip tags to tests.
</commit_message>
<xml_diff>
--- a/output/TestBook.xlsx
+++ b/output/TestBook.xlsx
@@ -7,9 +7,11 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="New Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Introduction_Modified" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="New Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="New Sheet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Introduction_Modified1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Introduction_Modified" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Sheet" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -441,6 +443,58 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="B1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>New Data</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>New Data</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -453,7 +507,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
Modified the function name Insert Cell value to Set Cell Value.
</commit_message>
<xml_diff>
--- a/output/TestBook.xlsx
+++ b/output/TestBook.xlsx
@@ -7,11 +7,13 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="New Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="New Sheet" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Introduction_Modified1" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Introduction_Modified" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Sheet" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="New Sheet3" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="New Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="New Sheet1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="New Sheet" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Introduction_Modified1" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Introduction_Modified" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Sheet" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -443,6 +445,24 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="B1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -463,7 +483,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -489,7 +509,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>New Data</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -507,7 +553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
Updated the Get cell value function call.
</commit_message>
<xml_diff>
--- a/output/TestBook.xlsx
+++ b/output/TestBook.xlsx
@@ -7,13 +7,15 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="New Sheet3" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="New Sheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="New Sheet1" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="New Sheet" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Introduction_Modified1" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Introduction_Modified" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Sheet" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="New Sheet5" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="New Sheet4" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="New Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="New Sheet2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="New Sheet1" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="New Sheet" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Introduction_Modified1" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Introduction_Modified" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Sheet" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -445,24 +447,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="B1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -483,7 +467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -509,6 +493,24 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -541,6 +543,58 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="B1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>New Data</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>New Data</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -553,7 +607,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
Updated the docs for new functions added.
</commit_message>
<xml_diff>
--- a/output/TestBook.xlsx
+++ b/output/TestBook.xlsx
@@ -7,15 +7,16 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="New Sheet5" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="New Sheet4" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="New Sheet3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="New Sheet2" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="New Sheet1" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="New Sheet" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Introduction_Modified1" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Introduction_Modified" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Sheet" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="New Sheet6" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="New Sheet5" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="New Sheet4" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="New Sheet3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="New Sheet2" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="New Sheet1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="New Sheet" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Introduction_Modified1" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Introduction_Modified" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Sheet" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -441,6 +442,24 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -499,24 +518,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="B1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -537,6 +538,24 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -595,6 +614,32 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="B1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>New Data</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -605,22 +650,4 @@
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Insert Row and Column of List data.
</commit_message>
<xml_diff>
--- a/output/TestBook.xlsx
+++ b/output/TestBook.xlsx
@@ -7,16 +7,17 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="New Sheet6" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="New Sheet5" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="New Sheet4" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="New Sheet3" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="New Sheet2" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="New Sheet1" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="New Sheet" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Introduction_Modified1" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Introduction_Modified" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Sheet" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="New Sheet7" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="New Sheet6" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="New Sheet5" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="New Sheet4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="New Sheet3" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="New Sheet2" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="New Sheet1" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="New Sheet" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Introduction_Modified1" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Introduction_Modified" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Sheet" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -460,6 +461,24 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -544,6 +563,32 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="B1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>New Data</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -556,32 +601,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="B1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>New Data</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -640,14 +659,22 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <dimension ref="B1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>New Data</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>